<commit_message>
fixed (for real this time)
</commit_message>
<xml_diff>
--- a/test/writer_output/Dual Mode Desorption.xlsx
+++ b/test/writer_output/Dual Mode Desorption.xlsx
@@ -462,22 +462,22 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>71.32860750316964</v>
+        <v>71.32860750403187</v>
       </c>
       <c r="C2">
-        <v>2.6288621100915446</v>
+        <v>2.628862110231255</v>
       </c>
       <c r="D2">
-        <v>5.324287870037927</v>
+        <v>5.324287869830096</v>
       </c>
       <c r="E2">
-        <v>0.4678058647134821</v>
+        <v>0.4678058647411829</v>
       </c>
       <c r="F2">
-        <v>15.677832635940558</v>
+        <v>15.677832635673393</v>
       </c>
       <c r="G2">
-        <v>1.017720882402575</v>
+        <v>1.0177208824427562</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -485,22 +485,22 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>107.00819993075713</v>
+        <v>107.00819993220986</v>
       </c>
       <c r="C3">
-        <v>3.4575727046584115</v>
+        <v>3.457572705065848</v>
       </c>
       <c r="D3">
-        <v>5.324287870037927</v>
+        <v>5.324287869830096</v>
       </c>
       <c r="E3">
-        <v>0.4678058647134821</v>
+        <v>0.4678058647411829</v>
       </c>
       <c r="F3">
-        <v>4.5370386534270555</v>
+        <v>4.537038653148481</v>
       </c>
       <c r="G3">
-        <v>0.9449719631200497</v>
+        <v>0.9449719632663334</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -508,10 +508,10 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-50.02143414337928</v>
+        <v>-50.021434143602484</v>
       </c>
       <c r="C4">
-        <v>7.353129071185884</v>
+        <v>7.353129071700697</v>
       </c>
       <c r="D4">
         <v>0.0</v>
@@ -520,10 +520,10 @@
         <v>0.0</v>
       </c>
       <c r="F4">
-        <v>71.06080439316499</v>
+        <v>71.06080439444871</v>
       </c>
       <c r="G4">
-        <v>6.313405339461436</v>
+        <v>6.313405340457094</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -568,40 +568,22 @@
       <c r="E8">
         <v>0.0</v>
       </c>
-      <c r="F8">
-        <v>0.241333352</v>
-      </c>
-      <c r="G8">
-        <v>41.48924079</v>
-      </c>
-      <c r="H8">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
         <v>0.10836838037931033</v>
       </c>
       <c r="B9">
-        <v>27.79657380333988</v>
+        <v>27.796573802980408</v>
       </c>
       <c r="C9">
-        <v>1.7468678134784517</v>
+        <v>1.7468678136146318</v>
       </c>
       <c r="D9">
-        <v>39.643654035067016</v>
+        <v>39.64365403459924</v>
       </c>
       <c r="E9">
-        <v>2.5237354988421288</v>
-      </c>
-      <c r="F9">
-        <v>0.600763584</v>
-      </c>
-      <c r="G9">
-        <v>62.79313671</v>
-      </c>
-      <c r="H9">
-        <v>0.0</v>
+        <v>2.5237354990928993</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -609,25 +591,16 @@
         <v>0.21673676075862067</v>
       </c>
       <c r="B10">
-        <v>41.61160397589148</v>
+        <v>41.61160397560299</v>
       </c>
       <c r="C10">
-        <v>2.112342023644102</v>
+        <v>2.112342023808027</v>
       </c>
       <c r="D10">
-        <v>58.31199579984316</v>
+        <v>58.31199579952216</v>
       </c>
       <c r="E10">
-        <v>2.9902764128910557</v>
-      </c>
-      <c r="F10">
-        <v>1.04806673</v>
-      </c>
-      <c r="G10">
-        <v>77.9590348</v>
-      </c>
-      <c r="H10">
-        <v>0.0</v>
+        <v>2.9902764132172552</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -635,25 +608,16 @@
         <v>0.325105141137931</v>
       </c>
       <c r="B11">
-        <v>50.30697746063494</v>
+        <v>50.30697746044838</v>
       </c>
       <c r="C11">
-        <v>2.236408339356231</v>
+        <v>2.23640833952066</v>
       </c>
       <c r="D11">
-        <v>69.2997551783521</v>
+        <v>69.29975517821288</v>
       </c>
       <c r="E11">
-        <v>3.1078461520624563</v>
-      </c>
-      <c r="F11">
-        <v>1.466095481</v>
-      </c>
-      <c r="G11">
-        <v>88.08019013</v>
-      </c>
-      <c r="H11">
-        <v>0.0</v>
+        <v>3.1078461524145085</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -661,25 +625,16 @@
         <v>0.43347352151724133</v>
       </c>
       <c r="B12">
-        <v>56.56167053978254</v>
+        <v>56.561670539681046</v>
       </c>
       <c r="C12">
-        <v>2.3034686836304337</v>
+        <v>2.3034686837895526</v>
       </c>
       <c r="D12">
-        <v>76.62597080952969</v>
+        <v>76.6259708095415</v>
       </c>
       <c r="E12">
-        <v>3.149538654378189</v>
-      </c>
-      <c r="F12">
-        <v>1.951571285</v>
-      </c>
-      <c r="G12">
-        <v>96.61909374</v>
-      </c>
-      <c r="H12">
-        <v>0.0</v>
+        <v>3.1495386547412543</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -687,25 +642,16 @@
         <v>0.5418419018965517</v>
       </c>
       <c r="B13">
-        <v>61.463144855656964</v>
+        <v>61.46314485562027</v>
       </c>
       <c r="C13">
-        <v>2.3558793453584523</v>
+        <v>2.355879345512013</v>
       </c>
       <c r="D13">
-        <v>81.92206824494754</v>
+        <v>81.92206824507697</v>
       </c>
       <c r="E13">
-        <v>3.1756026772111</v>
-      </c>
-      <c r="F13">
-        <v>2.499847618</v>
-      </c>
-      <c r="G13">
-        <v>105.7659302</v>
-      </c>
-      <c r="H13">
-        <v>0.0</v>
+        <v>3.175602677580648</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -713,25 +659,16 @@
         <v>0.650210282275862</v>
       </c>
       <c r="B14">
-        <v>65.53636847951702</v>
+        <v>65.53636847952815</v>
       </c>
       <c r="C14">
-        <v>2.405376496831536</v>
+        <v>2.4053764969806233</v>
       </c>
       <c r="D14">
-        <v>85.97561211390303</v>
+        <v>85.9756121141227</v>
       </c>
       <c r="E14">
-        <v>3.2011185765377443</v>
-      </c>
-      <c r="F14">
-        <v>3.142683031</v>
-      </c>
-      <c r="G14">
-        <v>114.9523482</v>
-      </c>
-      <c r="H14">
-        <v>0.0</v>
+        <v>3.201118576912614</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -739,25 +676,16 @@
         <v>0.7585786626551724</v>
       </c>
       <c r="B15">
-        <v>69.06586101475506</v>
+        <v>69.06586101480062</v>
       </c>
       <c r="C15">
-        <v>2.455592966347851</v>
+        <v>2.4555929664937044</v>
       </c>
       <c r="D15">
-        <v>89.2134428058243</v>
+        <v>89.21344280611297</v>
       </c>
       <c r="E15">
-        <v>3.2297498028576306</v>
-      </c>
-      <c r="F15">
-        <v>2.60974313</v>
-      </c>
-      <c r="G15">
-        <v>111.9833899</v>
-      </c>
-      <c r="H15">
-        <v>0.0</v>
+        <v>3.2297498032378162</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -765,25 +693,16 @@
         <v>0.8669470430344827</v>
       </c>
       <c r="B16">
-        <v>72.21921398534715</v>
+        <v>72.21921398541672</v>
       </c>
       <c r="C16">
-        <v>2.507718969462108</v>
+        <v>2.5077189696058184</v>
       </c>
       <c r="D16">
-        <v>91.88698352848307</v>
+        <v>91.88698352882426</v>
       </c>
       <c r="E16">
-        <v>3.262067751841692</v>
-      </c>
-      <c r="F16">
-        <v>1.199714642</v>
-      </c>
-      <c r="G16">
-        <v>98.93545196</v>
-      </c>
-      <c r="H16">
-        <v>0.0</v>
+        <v>3.2620677522275856</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -791,25 +710,16 @@
         <v>0.9753154234137931</v>
       </c>
       <c r="B17">
-        <v>75.1015613737842</v>
+        <v>75.10156137386961</v>
       </c>
       <c r="C17">
-        <v>2.5621387721158246</v>
+        <v>2.5621387722582822</v>
       </c>
       <c r="D17">
-        <v>94.15395779018424</v>
+        <v>94.15395779056509</v>
       </c>
       <c r="E17">
-        <v>3.2978440494761654</v>
-      </c>
-      <c r="F17">
-        <v>0.575992209</v>
-      </c>
-      <c r="G17">
-        <v>81.21343867</v>
-      </c>
-      <c r="H17">
-        <v>0.0</v>
+        <v>3.297844049868267</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -817,25 +727,16 @@
         <v>1.0836838037931034</v>
       </c>
       <c r="B18">
-        <v>77.78219546893311</v>
+        <v>77.78219546902793</v>
       </c>
       <c r="C18">
-        <v>2.6189514678194965</v>
+        <v>2.6189514679614136</v>
       </c>
       <c r="D18">
-        <v>96.1183188764367</v>
+        <v>96.1183188768471</v>
       </c>
       <c r="E18">
-        <v>3.336706511902431</v>
-      </c>
-      <c r="F18">
-        <v>0.30991402</v>
-      </c>
-      <c r="G18">
-        <v>66.62816092</v>
-      </c>
-      <c r="H18">
-        <v>0.0</v>
+        <v>3.3367065123012583</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -843,25 +744,16 @@
         <v>1.1920521841724137</v>
       </c>
       <c r="B19">
-        <v>80.30864103329924</v>
+        <v>80.30864103339823</v>
       </c>
       <c r="C19">
-        <v>2.6781484824916664</v>
+        <v>2.6781484826336133</v>
       </c>
       <c r="D19">
-        <v>97.85136411752421</v>
+        <v>97.851364117956</v>
       </c>
       <c r="E19">
-        <v>3.378316462733599</v>
-      </c>
-      <c r="F19">
-        <v>0.145032338</v>
-      </c>
-      <c r="G19">
-        <v>50.92125421</v>
-      </c>
-      <c r="H19">
-        <v>0.0</v>
+        <v>3.3783164631396496</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -869,16 +761,16 @@
         <v>1.300420564551724</v>
       </c>
       <c r="B20">
-        <v>82.7145804797059</v>
+        <v>82.71458047980485</v>
       </c>
       <c r="C20">
-        <v>2.7396774179976093</v>
+        <v>2.739677418140044</v>
       </c>
       <c r="D20">
-        <v>99.40362435221847</v>
+        <v>99.40362435266498</v>
       </c>
       <c r="E20">
-        <v>3.422403052613224</v>
+        <v>3.4224030530269642</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -886,16 +778,16 @@
         <v>1.4087889449310345</v>
       </c>
       <c r="B21">
-        <v>85.02455156006677</v>
+        <v>85.02455156016218</v>
       </c>
       <c r="C21">
-        <v>2.8034662569374844</v>
+        <v>2.8034662570807813</v>
       </c>
       <c r="D21">
-        <v>100.8119114678468</v>
+        <v>100.81191146830261</v>
       </c>
       <c r="E21">
-        <v>3.468757369065459</v>
+        <v>3.4687573694873226</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -903,16 +795,16 @@
         <v>1.5171573253103448</v>
       </c>
       <c r="B22">
-        <v>87.25685354168203</v>
+        <v>87.25685354177102</v>
       </c>
       <c r="C22">
-        <v>2.8694332322706617</v>
+        <v>2.8694332324151297</v>
       </c>
       <c r="D22">
-        <v>102.10367828765077</v>
+        <v>102.10367828811138</v>
       </c>
       <c r="E22">
-        <v>3.517218157850368</v>
+        <v>3.517218158280758</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -920,16 +812,16 @@
         <v>1.625525705689655</v>
       </c>
       <c r="B23">
-        <v>89.42541131680673</v>
+        <v>89.42541131688685</v>
       </c>
       <c r="C23">
-        <v>2.9374913630279944</v>
+        <v>2.937491363173893</v>
       </c>
       <c r="D23">
-        <v>103.29981513469426</v>
+        <v>103.29981513515587</v>
       </c>
       <c r="E23">
-        <v>3.5676584359851042</v>
+        <v>3.5676584364243986</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -937,16 +829,16 @@
         <v>1.7338940860689653</v>
       </c>
       <c r="B24">
-        <v>91.54100879189735</v>
+        <v>91.54100879196655</v>
       </c>
       <c r="C24">
-        <v>3.0075509329366557</v>
+        <v>3.0075509330842056</v>
       </c>
       <c r="D24">
-        <v>104.4165001801</v>
+        <v>104.41650018055938</v>
       </c>
       <c r="E24">
-        <v>3.61997508420242</v>
+        <v>3.6199750846509713</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -954,16 +846,16 @@
         <v>1.8422624664482758</v>
       </c>
       <c r="B25">
-        <v>93.61212723726854</v>
+        <v>93.61212723732505</v>
       </c>
       <c r="C25">
-        <v>3.079521114172006</v>
+        <v>3.0795211143213974</v>
       </c>
       <c r="D25">
-        <v>105.46645714722759</v>
+        <v>105.46645714768202</v>
       </c>
       <c r="E25">
-        <v>3.6740813380681665</v>
+        <v>3.6740813385263045</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -971,16 +863,16 @@
         <v>1.9506308468275861</v>
       </c>
       <c r="B26">
-        <v>95.64552873075624</v>
+        <v>95.64552873079853</v>
       </c>
       <c r="C26">
-        <v>3.153311175625536</v>
+        <v>3.153311175776935</v>
       </c>
       <c r="D26">
-        <v>106.45983060222441</v>
+        <v>106.4598306026715</v>
       </c>
       <c r="E26">
-        <v>3.7299015738133563</v>
+        <v>3.7299015742813917</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -988,16 +880,16 @@
         <v>2.0589992272068964</v>
       </c>
       <c r="B27">
-        <v>97.64667075766167</v>
+        <v>97.64667075768844</v>
       </c>
       <c r="C27">
-        <v>3.228831436176389</v>
+        <v>3.228831436329941</v>
       </c>
       <c r="D27">
-        <v>107.40480794280748</v>
+        <v>107.40480794324522</v>
       </c>
       <c r="E27">
-        <v>3.7873677729688735</v>
+        <v>3.7873677734470985</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1005,16 +897,16 @@
         <v>2.1673676075862067</v>
       </c>
       <c r="B28">
-        <v>99.62000634961697</v>
+        <v>99.62000634962705</v>
       </c>
       <c r="C28">
-        <v>3.3059940247732307</v>
+        <v>3.3059940249290665</v>
       </c>
       <c r="D28">
-        <v>108.30806967089423</v>
+        <v>108.3080696713208</v>
       </c>
       <c r="E28">
-        <v>3.846417169088976</v>
+        <v>3.8464171695776668</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1022,16 +914,16 @@
         <v>2.275735987965517</v>
       </c>
       <c r="B29">
-        <v>101.56920500727193</v>
+        <v>101.56920500726434</v>
       </c>
       <c r="C29">
-        <v>3.3847134767346754</v>
+        <v>3.384713476892912</v>
       </c>
       <c r="D29">
-        <v>109.17512082398538</v>
+        <v>109.17512082439923</v>
       </c>
       <c r="E29">
-        <v>3.90699070892839</v>
+        <v>3.9069907094278054</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1039,16 +931,16 @@
         <v>2.3841043683448273</v>
       </c>
       <c r="B30">
-        <v>103.497317771306</v>
+        <v>103.49731777127985</v>
       </c>
       <c r="C30">
-        <v>3.464907186516097</v>
+        <v>3.4649071866768404</v>
       </c>
       <c r="D30">
-        <v>110.01053861706451</v>
+        <v>110.01053861746425</v>
       </c>
       <c r="E30">
-        <v>3.9690320665754255</v>
+        <v>3.9690320670858106</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1056,16 +948,16 @@
         <v>2.4924727487241376</v>
       </c>
       <c r="B31">
-        <v>105.40690224896062</v>
+        <v>105.4069022489151</v>
       </c>
       <c r="C31">
-        <v>3.5464957352445334</v>
+        <v>3.54649573540788</v>
       </c>
       <c r="D31">
-        <v>110.818160009195</v>
+        <v>110.8181600095794</v>
       </c>
       <c r="E31">
-        <v>4.032487028337963</v>
+        <v>4.032487028859549</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1073,16 +965,16 @@
         <v>2.600841129103448</v>
       </c>
       <c r="B32">
-        <v>107.30011848909896</v>
+        <v>107.3001184890334</v>
       </c>
       <c r="C32">
-        <v>3.6294031109271594</v>
+        <v>3.6294031110931977</v>
       </c>
       <c r="D32">
-        <v>111.60122553665958</v>
+        <v>111.60122553702757</v>
       </c>
       <c r="E32">
-        <v>4.097303122920519</v>
+        <v>4.097303123453523</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1090,16 +982,16 @@
         <v>2.7092095094827586</v>
       </c>
       <c r="B33">
-        <v>109.17880333902391</v>
+        <v>109.17880333893764</v>
       </c>
       <c r="C33">
-        <v>3.7135568386449713</v>
+        <v>3.7135568388137825</v>
       </c>
       <c r="D33">
-        <v>112.36249086412505</v>
+        <v>112.36249086447563</v>
       </c>
       <c r="E33">
-        <v>4.163429411178704</v>
+        <v>4.163429411723335</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1107,16 +999,16 @@
         <v>2.817577889862069</v>
       </c>
       <c r="B34">
-        <v>111.0445287143775</v>
+        <v>111.04452871426997</v>
       </c>
       <c r="C34">
-        <v>3.7988880369141826</v>
+        <v>3.7988880370858413</v>
       </c>
       <c r="D34">
-        <v>113.10431420198111</v>
+        <v>113.10431420231342</v>
       </c>
       <c r="E34">
-        <v>4.230816377280599</v>
+        <v>4.230816377837049</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1124,16 +1016,16 @@
         <v>2.925946270241379</v>
       </c>
       <c r="B35">
-        <v>112.89864770123394</v>
+        <v>112.89864770110462</v>
       </c>
       <c r="C35">
-        <v>3.885331414842333</v>
+        <v>3.885331415016909</v>
       </c>
       <c r="D35">
-        <v>113.82872546936149</v>
+        <v>113.82872546967474</v>
       </c>
       <c r="E35">
-        <v>4.299415882083086</v>
+        <v>4.299415882651538</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1141,16 +1033,16 @@
         <v>3.0343146506206895</v>
       </c>
       <c r="B36">
-        <v>114.74233135502189</v>
+        <v>114.74233135487037</v>
       </c>
       <c r="C36">
-        <v>3.972825222924756</v>
+        <v>3.9728252231023147</v>
       </c>
       <c r="D36">
-        <v>114.53748150041491</v>
+        <v>114.53748150070838</v>
       </c>
       <c r="E36">
-        <v>4.369181152566588</v>
+        <v>4.369181153147218</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1158,16 +1050,16 @@
         <v>3.142683031</v>
       </c>
       <c r="B37">
-        <v>116.5765983152324</v>
+        <v>116.57659831505822</v>
       </c>
       <c r="C37">
-        <v>4.061311168494988</v>
+        <v>4.061311168675589</v>
       </c>
       <c r="D37">
-        <v>115.23211047271452</v>
+        <v>115.2321104729876</v>
       </c>
       <c r="E37">
-        <v>4.440066790103542</v>
+        <v>4.440066790696512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version; added custom density option for nelf
</commit_message>
<xml_diff>
--- a/test/writer_output/Dual Mode Desorption.xlsx
+++ b/test/writer_output/Dual Mode Desorption.xlsx
@@ -568,6 +568,15 @@
       <c r="E8">
         <v>0.0</v>
       </c>
+      <c r="F8">
+        <v>0.241333352</v>
+      </c>
+      <c r="G8">
+        <v>41.48924079</v>
+      </c>
+      <c r="H8">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
@@ -585,6 +594,15 @@
       <c r="E9">
         <v>2.5237354990928993</v>
       </c>
+      <c r="F9">
+        <v>0.600763584</v>
+      </c>
+      <c r="G9">
+        <v>62.79313671</v>
+      </c>
+      <c r="H9">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
@@ -602,6 +620,15 @@
       <c r="E10">
         <v>2.9902764132172552</v>
       </c>
+      <c r="F10">
+        <v>1.04806673</v>
+      </c>
+      <c r="G10">
+        <v>77.9590348</v>
+      </c>
+      <c r="H10">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
@@ -619,6 +646,15 @@
       <c r="E11">
         <v>3.1078461524145085</v>
       </c>
+      <c r="F11">
+        <v>1.466095481</v>
+      </c>
+      <c r="G11">
+        <v>88.08019013</v>
+      </c>
+      <c r="H11">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
@@ -636,6 +672,15 @@
       <c r="E12">
         <v>3.1495386547412543</v>
       </c>
+      <c r="F12">
+        <v>1.951571285</v>
+      </c>
+      <c r="G12">
+        <v>96.61909374</v>
+      </c>
+      <c r="H12">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
@@ -653,6 +698,15 @@
       <c r="E13">
         <v>3.175602677580648</v>
       </c>
+      <c r="F13">
+        <v>2.499847618</v>
+      </c>
+      <c r="G13">
+        <v>105.7659302</v>
+      </c>
+      <c r="H13">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
@@ -670,6 +724,15 @@
       <c r="E14">
         <v>3.201118576912614</v>
       </c>
+      <c r="F14">
+        <v>3.142683031</v>
+      </c>
+      <c r="G14">
+        <v>114.9523482</v>
+      </c>
+      <c r="H14">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
@@ -687,6 +750,15 @@
       <c r="E15">
         <v>3.2297498032378162</v>
       </c>
+      <c r="F15">
+        <v>2.60974313</v>
+      </c>
+      <c r="G15">
+        <v>111.9833899</v>
+      </c>
+      <c r="H15">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
@@ -704,6 +776,15 @@
       <c r="E16">
         <v>3.2620677522275856</v>
       </c>
+      <c r="F16">
+        <v>1.199714642</v>
+      </c>
+      <c r="G16">
+        <v>98.93545196</v>
+      </c>
+      <c r="H16">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
@@ -721,6 +802,15 @@
       <c r="E17">
         <v>3.297844049868267</v>
       </c>
+      <c r="F17">
+        <v>0.575992209</v>
+      </c>
+      <c r="G17">
+        <v>81.21343867</v>
+      </c>
+      <c r="H17">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
@@ -738,6 +828,15 @@
       <c r="E18">
         <v>3.3367065123012583</v>
       </c>
+      <c r="F18">
+        <v>0.30991402</v>
+      </c>
+      <c r="G18">
+        <v>66.62816092</v>
+      </c>
+      <c r="H18">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
@@ -754,6 +853,15 @@
       </c>
       <c r="E19">
         <v>3.3783164631396496</v>
+      </c>
+      <c r="F19">
+        <v>0.145032338</v>
+      </c>
+      <c r="G19">
+        <v>50.92125421</v>
+      </c>
+      <c r="H19">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:8">

</xml_diff>

<commit_message>
fixed jackknife bug in dmds, new version
</commit_message>
<xml_diff>
--- a/test/writer_output/Dual Mode Desorption.xlsx
+++ b/test/writer_output/Dual Mode Desorption.xlsx
@@ -568,6 +568,15 @@
       <c r="E8">
         <v>0.0</v>
       </c>
+      <c r="F8">
+        <v>0.241333352</v>
+      </c>
+      <c r="G8">
+        <v>41.48924079</v>
+      </c>
+      <c r="H8">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
@@ -585,6 +594,15 @@
       <c r="E9">
         <v>2.5237354990928993</v>
       </c>
+      <c r="F9">
+        <v>0.600763584</v>
+      </c>
+      <c r="G9">
+        <v>62.79313671</v>
+      </c>
+      <c r="H9">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
@@ -602,6 +620,15 @@
       <c r="E10">
         <v>2.9902764132172552</v>
       </c>
+      <c r="F10">
+        <v>1.04806673</v>
+      </c>
+      <c r="G10">
+        <v>77.9590348</v>
+      </c>
+      <c r="H10">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
@@ -619,6 +646,15 @@
       <c r="E11">
         <v>3.1078461524145085</v>
       </c>
+      <c r="F11">
+        <v>1.466095481</v>
+      </c>
+      <c r="G11">
+        <v>88.08019013</v>
+      </c>
+      <c r="H11">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
@@ -636,6 +672,15 @@
       <c r="E12">
         <v>3.1495386547412543</v>
       </c>
+      <c r="F12">
+        <v>1.951571285</v>
+      </c>
+      <c r="G12">
+        <v>96.61909374</v>
+      </c>
+      <c r="H12">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
@@ -653,6 +698,15 @@
       <c r="E13">
         <v>3.175602677580648</v>
       </c>
+      <c r="F13">
+        <v>2.499847618</v>
+      </c>
+      <c r="G13">
+        <v>105.7659302</v>
+      </c>
+      <c r="H13">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
@@ -670,6 +724,15 @@
       <c r="E14">
         <v>3.201118576912614</v>
       </c>
+      <c r="F14">
+        <v>3.142683031</v>
+      </c>
+      <c r="G14">
+        <v>114.9523482</v>
+      </c>
+      <c r="H14">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
@@ -687,6 +750,15 @@
       <c r="E15">
         <v>3.2297498032378162</v>
       </c>
+      <c r="F15">
+        <v>2.60974313</v>
+      </c>
+      <c r="G15">
+        <v>111.9833899</v>
+      </c>
+      <c r="H15">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
@@ -704,6 +776,15 @@
       <c r="E16">
         <v>3.2620677522275856</v>
       </c>
+      <c r="F16">
+        <v>1.199714642</v>
+      </c>
+      <c r="G16">
+        <v>98.93545196</v>
+      </c>
+      <c r="H16">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
@@ -721,6 +802,15 @@
       <c r="E17">
         <v>3.297844049868267</v>
       </c>
+      <c r="F17">
+        <v>0.575992209</v>
+      </c>
+      <c r="G17">
+        <v>81.21343867</v>
+      </c>
+      <c r="H17">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
@@ -738,6 +828,15 @@
       <c r="E18">
         <v>3.3367065123012583</v>
       </c>
+      <c r="F18">
+        <v>0.30991402</v>
+      </c>
+      <c r="G18">
+        <v>66.62816092</v>
+      </c>
+      <c r="H18">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
@@ -754,6 +853,15 @@
       </c>
       <c r="E19">
         <v>3.3783164631396496</v>
+      </c>
+      <c r="F19">
+        <v>0.145032338</v>
+      </c>
+      <c r="G19">
+        <v>50.92125421</v>
+      </c>
+      <c r="H19">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:8">

</xml_diff>

<commit_message>
dgrpt technically works, issues with apply weights in dual mode
</commit_message>
<xml_diff>
--- a/test/writer_output/Dual Mode Desorption.xlsx
+++ b/test/writer_output/Dual Mode Desorption.xlsx
@@ -462,22 +462,22 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>71.32860750403187</v>
+        <v>71.32860750316964</v>
       </c>
       <c r="C2">
-        <v>2.628862110231255</v>
+        <v>2.6288621100915446</v>
       </c>
       <c r="D2">
-        <v>5.324287869830096</v>
+        <v>5.324287870037927</v>
       </c>
       <c r="E2">
-        <v>0.4678058647411829</v>
+        <v>0.4678058647134821</v>
       </c>
       <c r="F2">
-        <v>15.677832635673393</v>
+        <v>15.677832635940558</v>
       </c>
       <c r="G2">
-        <v>1.0177208824427562</v>
+        <v>1.017720882402575</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -485,22 +485,22 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>107.00819993220986</v>
+        <v>107.00819993075713</v>
       </c>
       <c r="C3">
-        <v>3.457572705065848</v>
+        <v>3.4575727046584115</v>
       </c>
       <c r="D3">
-        <v>5.324287869830096</v>
+        <v>5.324287870037927</v>
       </c>
       <c r="E3">
-        <v>0.4678058647411829</v>
+        <v>0.4678058647134821</v>
       </c>
       <c r="F3">
-        <v>4.537038653148481</v>
+        <v>4.5370386534270555</v>
       </c>
       <c r="G3">
-        <v>0.9449719632663334</v>
+        <v>0.9449719631200497</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -508,10 +508,10 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-50.021434143602484</v>
+        <v>-50.02143414337928</v>
       </c>
       <c r="C4">
-        <v>7.353129071700697</v>
+        <v>7.353129071185884</v>
       </c>
       <c r="D4">
         <v>0.0</v>
@@ -520,10 +520,10 @@
         <v>0.0</v>
       </c>
       <c r="F4">
-        <v>71.06080439444871</v>
+        <v>71.06080439316499</v>
       </c>
       <c r="G4">
-        <v>6.313405340457094</v>
+        <v>6.313405339461436</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -583,16 +583,16 @@
         <v>0.10836838037931033</v>
       </c>
       <c r="B9">
-        <v>27.796573802980408</v>
+        <v>27.79657380333988</v>
       </c>
       <c r="C9">
-        <v>1.7468678136146318</v>
+        <v>1.7468678134784517</v>
       </c>
       <c r="D9">
-        <v>39.64365403459924</v>
+        <v>39.643654035067016</v>
       </c>
       <c r="E9">
-        <v>2.5237354990928993</v>
+        <v>2.5237354988421288</v>
       </c>
       <c r="F9">
         <v>0.600763584</v>
@@ -609,16 +609,16 @@
         <v>0.21673676075862067</v>
       </c>
       <c r="B10">
-        <v>41.61160397560299</v>
+        <v>41.61160397589148</v>
       </c>
       <c r="C10">
-        <v>2.112342023808027</v>
+        <v>2.112342023644102</v>
       </c>
       <c r="D10">
-        <v>58.31199579952216</v>
+        <v>58.31199579984316</v>
       </c>
       <c r="E10">
-        <v>2.9902764132172552</v>
+        <v>2.9902764128910557</v>
       </c>
       <c r="F10">
         <v>1.04806673</v>
@@ -635,16 +635,16 @@
         <v>0.325105141137931</v>
       </c>
       <c r="B11">
-        <v>50.30697746044838</v>
+        <v>50.30697746063494</v>
       </c>
       <c r="C11">
-        <v>2.23640833952066</v>
+        <v>2.236408339356231</v>
       </c>
       <c r="D11">
-        <v>69.29975517821288</v>
+        <v>69.2997551783521</v>
       </c>
       <c r="E11">
-        <v>3.1078461524145085</v>
+        <v>3.1078461520624563</v>
       </c>
       <c r="F11">
         <v>1.466095481</v>
@@ -661,16 +661,16 @@
         <v>0.43347352151724133</v>
       </c>
       <c r="B12">
-        <v>56.561670539681046</v>
+        <v>56.56167053978254</v>
       </c>
       <c r="C12">
-        <v>2.3034686837895526</v>
+        <v>2.3034686836304337</v>
       </c>
       <c r="D12">
-        <v>76.6259708095415</v>
+        <v>76.62597080952969</v>
       </c>
       <c r="E12">
-        <v>3.1495386547412543</v>
+        <v>3.149538654378189</v>
       </c>
       <c r="F12">
         <v>1.951571285</v>
@@ -687,16 +687,16 @@
         <v>0.5418419018965517</v>
       </c>
       <c r="B13">
-        <v>61.46314485562027</v>
+        <v>61.463144855656964</v>
       </c>
       <c r="C13">
-        <v>2.355879345512013</v>
+        <v>2.3558793453584523</v>
       </c>
       <c r="D13">
-        <v>81.92206824507697</v>
+        <v>81.92206824494754</v>
       </c>
       <c r="E13">
-        <v>3.175602677580648</v>
+        <v>3.1756026772111</v>
       </c>
       <c r="F13">
         <v>2.499847618</v>
@@ -713,16 +713,16 @@
         <v>0.650210282275862</v>
       </c>
       <c r="B14">
-        <v>65.53636847952815</v>
+        <v>65.53636847951702</v>
       </c>
       <c r="C14">
-        <v>2.4053764969806233</v>
+        <v>2.405376496831536</v>
       </c>
       <c r="D14">
-        <v>85.9756121141227</v>
+        <v>85.97561211390303</v>
       </c>
       <c r="E14">
-        <v>3.201118576912614</v>
+        <v>3.2011185765377443</v>
       </c>
       <c r="F14">
         <v>3.142683031</v>
@@ -739,16 +739,16 @@
         <v>0.7585786626551724</v>
       </c>
       <c r="B15">
-        <v>69.06586101480062</v>
+        <v>69.06586101475506</v>
       </c>
       <c r="C15">
-        <v>2.4555929664937044</v>
+        <v>2.455592966347851</v>
       </c>
       <c r="D15">
-        <v>89.21344280611297</v>
+        <v>89.2134428058243</v>
       </c>
       <c r="E15">
-        <v>3.2297498032378162</v>
+        <v>3.2297498028576306</v>
       </c>
       <c r="F15">
         <v>2.60974313</v>
@@ -765,16 +765,16 @@
         <v>0.8669470430344827</v>
       </c>
       <c r="B16">
-        <v>72.21921398541672</v>
+        <v>72.21921398534715</v>
       </c>
       <c r="C16">
-        <v>2.5077189696058184</v>
+        <v>2.507718969462108</v>
       </c>
       <c r="D16">
-        <v>91.88698352882426</v>
+        <v>91.88698352848307</v>
       </c>
       <c r="E16">
-        <v>3.2620677522275856</v>
+        <v>3.262067751841692</v>
       </c>
       <c r="F16">
         <v>1.199714642</v>
@@ -791,16 +791,16 @@
         <v>0.9753154234137931</v>
       </c>
       <c r="B17">
-        <v>75.10156137386961</v>
+        <v>75.1015613737842</v>
       </c>
       <c r="C17">
-        <v>2.5621387722582822</v>
+        <v>2.5621387721158246</v>
       </c>
       <c r="D17">
-        <v>94.15395779056509</v>
+        <v>94.15395779018424</v>
       </c>
       <c r="E17">
-        <v>3.297844049868267</v>
+        <v>3.2978440494761654</v>
       </c>
       <c r="F17">
         <v>0.575992209</v>
@@ -817,16 +817,16 @@
         <v>1.0836838037931034</v>
       </c>
       <c r="B18">
-        <v>77.78219546902793</v>
+        <v>77.78219546893311</v>
       </c>
       <c r="C18">
-        <v>2.6189514679614136</v>
+        <v>2.6189514678194965</v>
       </c>
       <c r="D18">
-        <v>96.1183188768471</v>
+        <v>96.1183188764367</v>
       </c>
       <c r="E18">
-        <v>3.3367065123012583</v>
+        <v>3.336706511902431</v>
       </c>
       <c r="F18">
         <v>0.30991402</v>
@@ -843,16 +843,16 @@
         <v>1.1920521841724137</v>
       </c>
       <c r="B19">
-        <v>80.30864103339823</v>
+        <v>80.30864103329924</v>
       </c>
       <c r="C19">
-        <v>2.6781484826336133</v>
+        <v>2.6781484824916664</v>
       </c>
       <c r="D19">
-        <v>97.851364117956</v>
+        <v>97.85136411752421</v>
       </c>
       <c r="E19">
-        <v>3.3783164631396496</v>
+        <v>3.378316462733599</v>
       </c>
       <c r="F19">
         <v>0.145032338</v>
@@ -869,16 +869,16 @@
         <v>1.300420564551724</v>
       </c>
       <c r="B20">
-        <v>82.71458047980485</v>
+        <v>82.7145804797059</v>
       </c>
       <c r="C20">
-        <v>2.739677418140044</v>
+        <v>2.7396774179976093</v>
       </c>
       <c r="D20">
-        <v>99.40362435266498</v>
+        <v>99.40362435221847</v>
       </c>
       <c r="E20">
-        <v>3.4224030530269642</v>
+        <v>3.422403052613224</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -886,16 +886,16 @@
         <v>1.4087889449310345</v>
       </c>
       <c r="B21">
-        <v>85.02455156016218</v>
+        <v>85.02455156006677</v>
       </c>
       <c r="C21">
-        <v>2.8034662570807813</v>
+        <v>2.8034662569374844</v>
       </c>
       <c r="D21">
-        <v>100.81191146830261</v>
+        <v>100.8119114678468</v>
       </c>
       <c r="E21">
-        <v>3.4687573694873226</v>
+        <v>3.468757369065459</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -903,16 +903,16 @@
         <v>1.5171573253103448</v>
       </c>
       <c r="B22">
-        <v>87.25685354177102</v>
+        <v>87.25685354168203</v>
       </c>
       <c r="C22">
-        <v>2.8694332324151297</v>
+        <v>2.8694332322706617</v>
       </c>
       <c r="D22">
-        <v>102.10367828811138</v>
+        <v>102.10367828765077</v>
       </c>
       <c r="E22">
-        <v>3.517218158280758</v>
+        <v>3.517218157850368</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -920,16 +920,16 @@
         <v>1.625525705689655</v>
       </c>
       <c r="B23">
-        <v>89.42541131688685</v>
+        <v>89.42541131680673</v>
       </c>
       <c r="C23">
-        <v>2.937491363173893</v>
+        <v>2.9374913630279944</v>
       </c>
       <c r="D23">
-        <v>103.29981513515587</v>
+        <v>103.29981513469426</v>
       </c>
       <c r="E23">
-        <v>3.5676584364243986</v>
+        <v>3.5676584359851042</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -937,16 +937,16 @@
         <v>1.7338940860689653</v>
       </c>
       <c r="B24">
-        <v>91.54100879196655</v>
+        <v>91.54100879189735</v>
       </c>
       <c r="C24">
-        <v>3.0075509330842056</v>
+        <v>3.0075509329366557</v>
       </c>
       <c r="D24">
-        <v>104.41650018055938</v>
+        <v>104.4165001801</v>
       </c>
       <c r="E24">
-        <v>3.6199750846509713</v>
+        <v>3.61997508420242</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -954,16 +954,16 @@
         <v>1.8422624664482758</v>
       </c>
       <c r="B25">
-        <v>93.61212723732505</v>
+        <v>93.61212723726854</v>
       </c>
       <c r="C25">
-        <v>3.0795211143213974</v>
+        <v>3.079521114172006</v>
       </c>
       <c r="D25">
-        <v>105.46645714768202</v>
+        <v>105.46645714722759</v>
       </c>
       <c r="E25">
-        <v>3.6740813385263045</v>
+        <v>3.6740813380681665</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -971,16 +971,16 @@
         <v>1.9506308468275861</v>
       </c>
       <c r="B26">
-        <v>95.64552873079853</v>
+        <v>95.64552873075624</v>
       </c>
       <c r="C26">
-        <v>3.153311175776935</v>
+        <v>3.153311175625536</v>
       </c>
       <c r="D26">
-        <v>106.4598306026715</v>
+        <v>106.45983060222441</v>
       </c>
       <c r="E26">
-        <v>3.7299015742813917</v>
+        <v>3.7299015738133563</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -988,16 +988,16 @@
         <v>2.0589992272068964</v>
       </c>
       <c r="B27">
-        <v>97.64667075768844</v>
+        <v>97.64667075766167</v>
       </c>
       <c r="C27">
-        <v>3.228831436329941</v>
+        <v>3.228831436176389</v>
       </c>
       <c r="D27">
-        <v>107.40480794324522</v>
+        <v>107.40480794280748</v>
       </c>
       <c r="E27">
-        <v>3.7873677734470985</v>
+        <v>3.7873677729688735</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1005,16 +1005,16 @@
         <v>2.1673676075862067</v>
       </c>
       <c r="B28">
-        <v>99.62000634962705</v>
+        <v>99.62000634961697</v>
       </c>
       <c r="C28">
-        <v>3.3059940249290665</v>
+        <v>3.3059940247732307</v>
       </c>
       <c r="D28">
-        <v>108.3080696713208</v>
+        <v>108.30806967089423</v>
       </c>
       <c r="E28">
-        <v>3.8464171695776668</v>
+        <v>3.846417169088976</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1022,16 +1022,16 @@
         <v>2.275735987965517</v>
       </c>
       <c r="B29">
-        <v>101.56920500726434</v>
+        <v>101.56920500727193</v>
       </c>
       <c r="C29">
-        <v>3.384713476892912</v>
+        <v>3.3847134767346754</v>
       </c>
       <c r="D29">
-        <v>109.17512082439923</v>
+        <v>109.17512082398538</v>
       </c>
       <c r="E29">
-        <v>3.9069907094278054</v>
+        <v>3.90699070892839</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1039,16 +1039,16 @@
         <v>2.3841043683448273</v>
       </c>
       <c r="B30">
-        <v>103.49731777127985</v>
+        <v>103.497317771306</v>
       </c>
       <c r="C30">
-        <v>3.4649071866768404</v>
+        <v>3.464907186516097</v>
       </c>
       <c r="D30">
-        <v>110.01053861746425</v>
+        <v>110.01053861706451</v>
       </c>
       <c r="E30">
-        <v>3.9690320670858106</v>
+        <v>3.9690320665754255</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1056,16 +1056,16 @@
         <v>2.4924727487241376</v>
       </c>
       <c r="B31">
-        <v>105.4069022489151</v>
+        <v>105.40690224896062</v>
       </c>
       <c r="C31">
-        <v>3.54649573540788</v>
+        <v>3.5464957352445334</v>
       </c>
       <c r="D31">
-        <v>110.8181600095794</v>
+        <v>110.818160009195</v>
       </c>
       <c r="E31">
-        <v>4.032487028859549</v>
+        <v>4.032487028337963</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1073,16 +1073,16 @@
         <v>2.600841129103448</v>
       </c>
       <c r="B32">
-        <v>107.3001184890334</v>
+        <v>107.30011848909896</v>
       </c>
       <c r="C32">
-        <v>3.6294031110931977</v>
+        <v>3.6294031109271594</v>
       </c>
       <c r="D32">
-        <v>111.60122553702757</v>
+        <v>111.60122553665958</v>
       </c>
       <c r="E32">
-        <v>4.097303123453523</v>
+        <v>4.097303122920519</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1090,16 +1090,16 @@
         <v>2.7092095094827586</v>
       </c>
       <c r="B33">
-        <v>109.17880333893764</v>
+        <v>109.17880333902391</v>
       </c>
       <c r="C33">
-        <v>3.7135568388137825</v>
+        <v>3.7135568386449713</v>
       </c>
       <c r="D33">
-        <v>112.36249086447563</v>
+        <v>112.36249086412505</v>
       </c>
       <c r="E33">
-        <v>4.163429411723335</v>
+        <v>4.163429411178704</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1107,16 +1107,16 @@
         <v>2.817577889862069</v>
       </c>
       <c r="B34">
-        <v>111.04452871426997</v>
+        <v>111.0445287143775</v>
       </c>
       <c r="C34">
-        <v>3.7988880370858413</v>
+        <v>3.7988880369141826</v>
       </c>
       <c r="D34">
-        <v>113.10431420231342</v>
+        <v>113.10431420198111</v>
       </c>
       <c r="E34">
-        <v>4.230816377837049</v>
+        <v>4.230816377280599</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1124,16 +1124,16 @@
         <v>2.925946270241379</v>
       </c>
       <c r="B35">
-        <v>112.89864770110462</v>
+        <v>112.89864770123394</v>
       </c>
       <c r="C35">
-        <v>3.885331415016909</v>
+        <v>3.885331414842333</v>
       </c>
       <c r="D35">
-        <v>113.82872546967474</v>
+        <v>113.82872546936149</v>
       </c>
       <c r="E35">
-        <v>4.299415882651538</v>
+        <v>4.299415882083086</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1141,16 +1141,16 @@
         <v>3.0343146506206895</v>
       </c>
       <c r="B36">
-        <v>114.74233135487037</v>
+        <v>114.74233135502189</v>
       </c>
       <c r="C36">
-        <v>3.9728252231023147</v>
+        <v>3.972825222924756</v>
       </c>
       <c r="D36">
-        <v>114.53748150070838</v>
+        <v>114.53748150041491</v>
       </c>
       <c r="E36">
-        <v>4.369181153147218</v>
+        <v>4.369181152566588</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1158,16 +1158,16 @@
         <v>3.142683031</v>
       </c>
       <c r="B37">
-        <v>116.57659831505822</v>
+        <v>116.5765983152324</v>
       </c>
       <c r="C37">
-        <v>4.061311168675589</v>
+        <v>4.061311168494988</v>
       </c>
       <c r="D37">
-        <v>115.2321104729876</v>
+        <v>115.23211047271452</v>
       </c>
       <c r="E37">
-        <v>4.440066790696512</v>
+        <v>4.440066790103542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>